<commit_message>
add new assets sheet for testing
</commit_message>
<xml_diff>
--- a/UnityProject/Assets/Samples/002 - Import From Excel/Excel/Heroes.xlsx
+++ b/UnityProject/Assets/Samples/002 - Import From Excel/Excel/Heroes.xlsx
@@ -1,17 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25721"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_BAF861E3230DD907CEC46E5CD38C34F2274DE0B5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Heroes" sheetId="1" r:id="rId4"/>
+    <sheet name="Heroes" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Id</t>
   </si>
@@ -67,28 +84,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -235,54 +239,54 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -293,27 +297,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -515,7 +577,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -534,7 +596,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -564,7 +626,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -590,7 +652,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -616,7 +678,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -642,7 +704,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -668,7 +730,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -694,7 +756,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -720,7 +782,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -746,7 +808,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -772,7 +834,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -785,9 +847,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -804,7 +872,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -823,7 +891,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -849,7 +917,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -875,7 +943,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -901,7 +969,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -927,7 +995,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -953,7 +1021,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -979,7 +1047,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1005,7 +1073,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1031,7 +1099,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1057,7 +1125,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1070,9 +1138,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1086,7 +1160,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1105,7 +1179,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1135,7 +1209,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1161,7 +1235,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1187,7 +1261,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1213,7 +1287,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1239,7 +1313,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1265,7 +1339,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1291,7 +1365,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1317,7 +1391,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1343,7 +1417,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1356,61 +1430,67 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:IV22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="10" width="16.3516" style="1" customWidth="1"/>
-    <col min="11" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="256" width="16.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:10" ht="20.25" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="4">
+    <row r="2" spans="1:10" ht="20.25" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="6">
@@ -1432,7 +1512,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" ht="20.05" customHeight="1">
+    <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
@@ -1448,7 +1528,7 @@
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
+    <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
@@ -1464,7 +1544,7 @@
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
+    <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
@@ -1480,7 +1560,7 @@
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
+    <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
@@ -1492,17 +1572,17 @@
       <c r="G6" s="11">
         <v>100</v>
       </c>
-      <c r="H6" t="s" s="12">
+      <c r="H6" s="12" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="13">
+    <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s" s="14">
+      <c r="B7" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="11">
@@ -1524,7 +1604,7 @@
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
+    <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
@@ -1540,7 +1620,7 @@
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" ht="20.05" customHeight="1">
+    <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
@@ -1556,7 +1636,7 @@
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" ht="20.05" customHeight="1">
+    <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
@@ -1572,7 +1652,7 @@
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" ht="20.05" customHeight="1">
+    <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
@@ -1584,17 +1664,17 @@
       <c r="G11" s="11">
         <v>100</v>
       </c>
-      <c r="H11" t="s" s="12">
+      <c r="H11" s="12" t="s">
         <v>13</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="13">
+    <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s" s="14">
+      <c r="B12" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="11">
@@ -1616,7 +1696,7 @@
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" ht="20.05" customHeight="1">
+    <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
@@ -1632,7 +1712,7 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" ht="20.05" customHeight="1">
+    <row r="14" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
@@ -1648,7 +1728,7 @@
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" ht="20.05" customHeight="1">
+    <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10"/>
@@ -1664,7 +1744,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" ht="20.05" customHeight="1">
+    <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
@@ -1676,13 +1756,13 @@
       <c r="G16" s="11">
         <v>100</v>
       </c>
-      <c r="H16" t="s" s="12">
+      <c r="H16" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" ht="20.05" customHeight="1">
+    <row r="17" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
@@ -1694,7 +1774,7 @@
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" ht="20.05" customHeight="1">
+    <row r="18" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
@@ -1706,7 +1786,7 @@
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
     </row>
-    <row r="19" ht="20.05" customHeight="1">
+    <row r="19" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
@@ -1718,7 +1798,7 @@
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
     </row>
-    <row r="20" ht="20.05" customHeight="1">
+    <row r="20" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10"/>
@@ -1730,7 +1810,7 @@
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
     </row>
-    <row r="21" ht="20.05" customHeight="1">
+    <row r="21" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
@@ -1742,7 +1822,7 @@
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
     </row>
-    <row r="22" ht="20.05" customHeight="1">
+    <row r="22" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
@@ -1755,8 +1835,8 @@
       <c r="J22" s="10"/>
     </row>
   </sheetData>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup scale="72" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>